<commit_message>
avance activacion-inactivacion eprepago 24092019
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/e-prepago/activacion_eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/e-prepago/activacion_eprepago.xlsx
@@ -79,13 +79,13 @@
     <t>CONSULTAR_PRODUCTO</t>
   </si>
   <si>
-    <t>matrix01</t>
-  </si>
-  <si>
-    <t>6789</t>
-  </si>
-  <si>
-    <t>9876</t>
+    <t>pruebasregistro48</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>4321</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -547,7 +547,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="5">
-        <v>22483228</v>
+        <v>700100</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
ejecucion ok activacion eprepago
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/e-prepago/activacion_eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/e-prepago/activacion_eprepago.xlsx
@@ -79,13 +79,13 @@
     <t>CONSULTAR_PRODUCTO</t>
   </si>
   <si>
-    <t>pruebasregistro48</t>
-  </si>
-  <si>
     <t>1234</t>
   </si>
   <si>
     <t>4321</t>
+  </si>
+  <si>
+    <t>pruebasregistro49</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -547,19 +547,19 @@
         <v>13</v>
       </c>
       <c r="B2" s="5">
-        <v>700100</v>
+        <v>700101</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>14</v>

</xml_diff>